<commit_message>
Added week 2 activities
</commit_message>
<xml_diff>
--- a/src/tutorialpkg/data/paralympics_all_raw.xlsx
+++ b/src/tutorialpkg/data/paralympics_all_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0035-2024-tutorials/src/tutorialpkg/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{043E84FC-9DA6-954A-B318-92E2B28B3884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ABA991-ED7A-2649-BCE9-86A0DFB3A337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17200" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2667" uniqueCount="377">
   <si>
     <t>type</t>
   </si>
@@ -1162,6 +1162,12 @@
   </si>
   <si>
     <t>First summer games in France. The first time the Paralympic Opening Ceremony was held outside of a stadium</t>
+  </si>
+  <si>
+    <t>Summer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">winter </t>
   </si>
 </sst>
 </file>
@@ -1645,10 +1651,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2027,7 +2032,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2089,7 +2094,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>375</v>
       </c>
       <c r="B2">
         <v>1960</v>
@@ -2127,7 +2132,7 @@
       <c r="O2" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2177,7 +2182,7 @@
       <c r="O3" t="s">
         <v>22</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="P3" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2227,7 +2232,7 @@
       <c r="O4" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2277,7 +2282,7 @@
       <c r="O5" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="P5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2327,7 +2332,7 @@
       <c r="O6" t="s">
         <v>32</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="P6" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2427,7 +2432,7 @@
       <c r="O8" t="s">
         <v>39</v>
       </c>
-      <c r="P8" s="2" t="s">
+      <c r="P8" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2477,7 +2482,7 @@
       <c r="O9" t="s">
         <v>42</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="P9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2965,7 +2970,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>376</v>
       </c>
       <c r="B20">
         <v>1976</v>

</xml_diff>

<commit_message>
Moved week 8 code to a new package to avoid confusion and better support week 9 testing
</commit_message>
<xml_diff>
--- a/src/tutorialpkg/data/paralympics_all_raw.xlsx
+++ b/src/tutorialpkg/data/paralympics_all_raw.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarahsanders/PycharmProjects/comp0035-2024-tutorials/src/tutorialpkg/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D10F82A1-646F-E74E-987D-BC6ABA87BDD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE73406-6A13-9A45-B630-E37D9987502E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="760" windowWidth="28040" windowHeight="17200" xr2:uid="{CBF15B4E-2805-CD44-9DA6-567684115F1A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2666" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2666" uniqueCount="375">
   <si>
     <t>type</t>
   </si>
@@ -1159,9 +1159,6 @@
   </si>
   <si>
     <t>First summer games in France. The first time the Paralympic Opening Ceremony was held outside of a stadium</t>
-  </si>
-  <si>
-    <t>Summer</t>
   </si>
   <si>
     <t xml:space="preserve">winter </t>
@@ -2029,7 +2026,7 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2088,7 +2085,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>374</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>1960</v>
@@ -2910,7 +2907,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B20">
         <v>1976</v>

</xml_diff>